<commit_message>
Added function to check for errors. Next: including the program for Groot
</commit_message>
<xml_diff>
--- a/data/planning_2012_edit.xlsx
+++ b/data/planning_2012_edit.xlsx
@@ -370,9 +370,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
-    <numFmt formatCode="H:MM" numFmtId="165"/>
+    <numFmt formatCode="DD/MM/YY\ HH:MM" numFmtId="165"/>
+    <numFmt formatCode="H:MM" numFmtId="166"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -495,7 +496,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
@@ -518,10 +519,10 @@
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
+    <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="false" borderId="2" fillId="0" fontId="0" numFmtId="165" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="false" borderId="2" fillId="0" fontId="0" numFmtId="165" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="false" borderId="2" fillId="0" fontId="0" numFmtId="166" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
@@ -548,10 +549,7 @@
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="0" fontId="5" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="false" borderId="3" fillId="0" fontId="0" numFmtId="165" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="0" fontId="0" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="false" borderId="3" fillId="0" fontId="0" numFmtId="166" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="0" fontId="0" numFmtId="164" xfId="0">
@@ -593,14 +591,14 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="5.73725490196078"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="6.16862745098039"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="2" width="10.6117647058824"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="17.6392156862745"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="11.6156862745098"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="12.1921568627451"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="9.18039215686274"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="8.46274509803922"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="13.7019607843137"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="2" width="10.6980392156863"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="17.7843137254902"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="11.7176470588235"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="12.2901960784314"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="9.25882352941177"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="8.53333333333333"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.57647058823529"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="20" outlineLevel="0" r="1">
@@ -655,7 +653,7 @@
       <c r="H3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="I3" s="7" t="s">
         <v>10</v>
       </c>
       <c r="J3" s="1" t="s">
@@ -666,11 +664,11 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="4">
-      <c r="A4" s="9" t="n">
-        <v>0.395833333333333</v>
-      </c>
-      <c r="B4" s="9" t="n">
-        <v>0.416666666666667</v>
+      <c r="A4" s="8" t="n">
+        <v>41202.3958333333</v>
+      </c>
+      <c r="B4" s="8" t="n">
+        <v>41202.4166666667</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>11</v>
@@ -701,11 +699,11 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="5">
-      <c r="A5" s="9" t="n">
-        <v>0.416666666666667</v>
-      </c>
-      <c r="B5" s="9" t="n">
-        <v>0.4375</v>
+      <c r="A5" s="8" t="n">
+        <v>41202.4166666667</v>
+      </c>
+      <c r="B5" s="8" t="n">
+        <v>41202.4375</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>12</v>
@@ -736,11 +734,11 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="6">
-      <c r="A6" s="9" t="n">
-        <v>0.4375</v>
-      </c>
-      <c r="B6" s="9" t="n">
-        <v>0.458333333333333</v>
+      <c r="A6" s="8" t="n">
+        <v>41202.4375</v>
+      </c>
+      <c r="B6" s="8" t="n">
+        <v>41202.4583333333</v>
       </c>
       <c r="C6" s="11" t="s">
         <v>13</v>
@@ -765,11 +763,11 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="7">
-      <c r="A7" s="9" t="n">
-        <v>0.458333333333333</v>
-      </c>
-      <c r="B7" s="9" t="n">
-        <v>0.479166666666667</v>
+      <c r="A7" s="8" t="n">
+        <v>41202.4583333333</v>
+      </c>
+      <c r="B7" s="8" t="n">
+        <v>41202.4791666667</v>
       </c>
       <c r="C7" s="11" t="s">
         <v>17</v>
@@ -798,11 +796,11 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="8">
-      <c r="A8" s="9" t="n">
-        <v>0.479166666666667</v>
-      </c>
-      <c r="B8" s="9" t="n">
-        <v>0.5</v>
+      <c r="A8" s="8" t="n">
+        <v>41202.4791666667</v>
+      </c>
+      <c r="B8" s="8" t="n">
+        <v>41202.5</v>
       </c>
       <c r="C8" s="11" t="s">
         <v>18</v>
@@ -827,11 +825,11 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="9">
-      <c r="A9" s="9" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="B9" s="9" t="n">
-        <v>0.520833333333334</v>
+      <c r="A9" s="8" t="n">
+        <v>41202.5</v>
+      </c>
+      <c r="B9" s="8" t="n">
+        <v>41202.5208333333</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>21</v>
@@ -862,11 +860,11 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="10">
-      <c r="A10" s="9" t="n">
-        <v>0.520833333333333</v>
-      </c>
-      <c r="B10" s="9" t="n">
-        <v>0.541666666666667</v>
+      <c r="A10" s="8" t="n">
+        <v>41202.5208333333</v>
+      </c>
+      <c r="B10" s="8" t="n">
+        <v>41202.5416666667</v>
       </c>
       <c r="C10" s="11" t="n">
         <v>3</v>
@@ -897,11 +895,11 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="11">
-      <c r="A11" s="9" t="n">
-        <v>0.541666666666667</v>
-      </c>
-      <c r="B11" s="9" t="n">
-        <v>0.5625</v>
+      <c r="A11" s="8" t="n">
+        <v>41202.5416666667</v>
+      </c>
+      <c r="B11" s="8" t="n">
+        <v>41202.5625</v>
       </c>
       <c r="C11" s="11" t="n">
         <v>4</v>
@@ -926,11 +924,11 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="12">
-      <c r="A12" s="9" t="n">
-        <v>0.5625</v>
-      </c>
-      <c r="B12" s="9" t="n">
-        <v>0.583333333333334</v>
+      <c r="A12" s="8" t="n">
+        <v>41202.5625</v>
+      </c>
+      <c r="B12" s="8" t="n">
+        <v>41202.5833333333</v>
       </c>
       <c r="C12" s="11" t="n">
         <v>1</v>
@@ -959,11 +957,11 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="13">
-      <c r="A13" s="9" t="n">
-        <v>0.583333333333333</v>
-      </c>
-      <c r="B13" s="9" t="n">
-        <v>0.604166666666667</v>
+      <c r="A13" s="8" t="n">
+        <v>41202.5833333333</v>
+      </c>
+      <c r="B13" s="8" t="n">
+        <v>41202.6041666667</v>
       </c>
       <c r="C13" s="11" t="n">
         <v>2</v>
@@ -988,11 +986,11 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="14">
-      <c r="A14" s="9" t="n">
-        <v>0.604166666666667</v>
-      </c>
-      <c r="B14" s="9" t="n">
-        <v>0.625</v>
+      <c r="A14" s="8" t="n">
+        <v>41202.6041666667</v>
+      </c>
+      <c r="B14" s="8" t="n">
+        <v>41202.625</v>
       </c>
       <c r="C14" s="11" t="s">
         <v>23</v>
@@ -1023,11 +1021,11 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="15">
-      <c r="A15" s="9" t="n">
-        <v>0.625</v>
-      </c>
-      <c r="B15" s="9" t="n">
-        <v>0.645833333333333</v>
+      <c r="A15" s="8" t="n">
+        <v>41202.625</v>
+      </c>
+      <c r="B15" s="8" t="n">
+        <v>41202.6458333333</v>
       </c>
       <c r="C15" s="11" t="s">
         <v>25</v>
@@ -1052,11 +1050,11 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="16">
-      <c r="A16" s="9" t="n">
-        <v>0.645833333333333</v>
-      </c>
-      <c r="B16" s="9" t="n">
-        <v>0.666666666666667</v>
+      <c r="A16" s="8" t="n">
+        <v>41202.6458333333</v>
+      </c>
+      <c r="B16" s="8" t="n">
+        <v>41202.6666666667</v>
       </c>
       <c r="C16" s="11" t="s">
         <v>26</v>
@@ -1085,11 +1083,11 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="17">
-      <c r="A17" s="9" t="n">
-        <v>0.666666666666667</v>
-      </c>
-      <c r="B17" s="9" t="n">
-        <v>0.6875</v>
+      <c r="A17" s="8" t="n">
+        <v>41202.6666666667</v>
+      </c>
+      <c r="B17" s="8" t="n">
+        <v>41202.6875</v>
       </c>
       <c r="C17" s="11" t="s">
         <v>28</v>
@@ -1114,11 +1112,11 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="18">
-      <c r="A18" s="9" t="n">
-        <v>0.6875</v>
-      </c>
-      <c r="B18" s="9" t="n">
-        <v>0.708333333333333</v>
+      <c r="A18" s="8" t="n">
+        <v>41202.6875</v>
+      </c>
+      <c r="B18" s="8" t="n">
+        <v>41202.7083333333</v>
       </c>
       <c r="C18" s="12" t="s">
         <v>30</v>
@@ -1149,11 +1147,11 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="19">
-      <c r="A19" s="9" t="n">
-        <v>0.708333333333334</v>
-      </c>
-      <c r="B19" s="9" t="n">
-        <v>0.729166666666667</v>
+      <c r="A19" s="8" t="n">
+        <v>41202.7083333333</v>
+      </c>
+      <c r="B19" s="8" t="n">
+        <v>41202.7291666667</v>
       </c>
       <c r="C19" s="12" t="s">
         <v>30</v>
@@ -1184,11 +1182,11 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="20">
-      <c r="A20" s="9" t="n">
-        <v>0.729166666666667</v>
-      </c>
-      <c r="B20" s="9" t="n">
-        <v>0.75</v>
+      <c r="A20" s="8" t="n">
+        <v>41202.7291666667</v>
+      </c>
+      <c r="B20" s="8" t="n">
+        <v>41202.75</v>
       </c>
       <c r="C20" s="12" t="s">
         <v>31</v>
@@ -1219,11 +1217,11 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="21">
-      <c r="A21" s="9" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="B21" s="9" t="n">
-        <v>0.770833333333333</v>
+      <c r="A21" s="8" t="n">
+        <v>41202.75</v>
+      </c>
+      <c r="B21" s="8" t="n">
+        <v>41202.7708333333</v>
       </c>
       <c r="C21" s="12" t="s">
         <v>31</v>
@@ -1254,11 +1252,11 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="22">
-      <c r="A22" s="9" t="n">
-        <v>0.770833333333334</v>
-      </c>
-      <c r="B22" s="9" t="n">
-        <v>0.791666666666667</v>
+      <c r="A22" s="8" t="n">
+        <v>41202.7708333333</v>
+      </c>
+      <c r="B22" s="8" t="n">
+        <v>41202.7916666667</v>
       </c>
       <c r="C22" s="12" t="s">
         <v>32</v>
@@ -1289,11 +1287,11 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="23">
-      <c r="A23" s="9" t="n">
-        <v>0.791666666666667</v>
-      </c>
-      <c r="B23" s="9" t="n">
-        <v>0.8125</v>
+      <c r="A23" s="8" t="n">
+        <v>41202.7916666667</v>
+      </c>
+      <c r="B23" s="8" t="n">
+        <v>41202.8125</v>
       </c>
       <c r="C23" s="12" t="s">
         <v>32</v>
@@ -1324,11 +1322,11 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="24">
-      <c r="A24" s="9" t="n">
-        <v>0.8125</v>
-      </c>
-      <c r="B24" s="9" t="n">
-        <v>0.833333333333333</v>
+      <c r="A24" s="8" t="n">
+        <v>41202.8125</v>
+      </c>
+      <c r="B24" s="8" t="n">
+        <v>41202.8333333333</v>
       </c>
       <c r="C24" s="12" t="s">
         <v>33</v>
@@ -1359,11 +1357,11 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="25">
-      <c r="A25" s="9" t="n">
-        <v>0.833333333333334</v>
-      </c>
-      <c r="B25" s="9" t="n">
-        <v>0.854166666666667</v>
+      <c r="A25" s="8" t="n">
+        <v>41202.8333333333</v>
+      </c>
+      <c r="B25" s="8" t="n">
+        <v>41202.8541666667</v>
       </c>
       <c r="C25" s="12" t="s">
         <v>33</v>
@@ -1394,11 +1392,11 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="26">
-      <c r="A26" s="9" t="n">
-        <v>0.854166666666667</v>
-      </c>
-      <c r="B26" s="9" t="n">
-        <v>0.875</v>
+      <c r="A26" s="8" t="n">
+        <v>41202.8541666667</v>
+      </c>
+      <c r="B26" s="8" t="n">
+        <v>41202.875</v>
       </c>
       <c r="C26" s="12" t="s">
         <v>33</v>
@@ -1429,11 +1427,11 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="27">
-      <c r="A27" s="9" t="n">
-        <v>0.875000000000001</v>
-      </c>
-      <c r="B27" s="9" t="n">
-        <v>0.895833333333333</v>
+      <c r="A27" s="8" t="n">
+        <v>41202.875</v>
+      </c>
+      <c r="B27" s="8" t="n">
+        <v>41202.8958333333</v>
       </c>
       <c r="C27" s="12" t="s">
         <v>33</v>
@@ -1464,11 +1462,11 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="28">
-      <c r="A28" s="9" t="n">
-        <v>0.895833333333334</v>
-      </c>
-      <c r="B28" s="9" t="n">
-        <v>0.916666666666667</v>
+      <c r="A28" s="8" t="n">
+        <v>41202.8958333333</v>
+      </c>
+      <c r="B28" s="8" t="n">
+        <v>41202.9166666667</v>
       </c>
       <c r="C28" s="12" t="s">
         <v>34</v>
@@ -1499,11 +1497,11 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="29">
-      <c r="A29" s="9" t="n">
-        <v>0.916666666666667</v>
-      </c>
-      <c r="B29" s="9" t="n">
-        <v>0.9375</v>
+      <c r="A29" s="8" t="n">
+        <v>41202.9166666667</v>
+      </c>
+      <c r="B29" s="8" t="n">
+        <v>41202.9375</v>
       </c>
       <c r="C29" s="12" t="s">
         <v>35</v>
@@ -1534,11 +1532,11 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="30">
-      <c r="A30" s="9" t="n">
-        <v>0.937500000000001</v>
-      </c>
-      <c r="B30" s="9" t="n">
-        <v>0.958333333333333</v>
+      <c r="A30" s="8" t="n">
+        <v>41202.9375</v>
+      </c>
+      <c r="B30" s="8" t="n">
+        <v>41202.9583333333</v>
       </c>
       <c r="C30" s="12" t="s">
         <v>35</v>
@@ -1569,11 +1567,11 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="31">
-      <c r="A31" s="9" t="n">
-        <v>0.958333333333334</v>
-      </c>
-      <c r="B31" s="9" t="n">
-        <v>0.979166666666667</v>
+      <c r="A31" s="8" t="n">
+        <v>41202.9583333333</v>
+      </c>
+      <c r="B31" s="8" t="n">
+        <v>41202.9791666667</v>
       </c>
       <c r="C31" s="12" t="s">
         <v>36</v>
@@ -1604,11 +1602,11 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="32">
-      <c r="A32" s="9" t="n">
-        <v>0.979166666666667</v>
-      </c>
-      <c r="B32" s="9" t="n">
-        <v>1</v>
+      <c r="A32" s="8" t="n">
+        <v>41202.9791666667</v>
+      </c>
+      <c r="B32" s="8" t="n">
+        <v>41203</v>
       </c>
       <c r="C32" s="12" t="s">
         <v>36</v>
@@ -1672,10 +1670,12 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="35">
-      <c r="A35" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="B35" s="9"/>
+      <c r="A35" s="8" t="n">
+        <v>41203</v>
+      </c>
+      <c r="B35" s="8" t="n">
+        <v>41203.3125</v>
+      </c>
       <c r="C35" s="12" t="s">
         <v>36</v>
       </c>
@@ -1694,11 +1694,17 @@
       <c r="H35" s="9" t="n">
         <v>0</v>
       </c>
-      <c r="I35" s="9"/>
+      <c r="I35" s="9" t="n">
+        <v>-0.6875</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="36">
-      <c r="A36" s="9"/>
-      <c r="B36" s="9"/>
+      <c r="A36" s="8" t="n">
+        <v>41203</v>
+      </c>
+      <c r="B36" s="8" t="n">
+        <v>41203.3125</v>
+      </c>
       <c r="C36" s="12" t="s">
         <v>36</v>
       </c>
@@ -1714,13 +1720,19 @@
       <c r="G36" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="H36" s="9"/>
-      <c r="I36" s="9"/>
+      <c r="H36" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="I36" s="9" t="n">
+        <v>0.3125</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="37">
-      <c r="A37" s="9"/>
-      <c r="B37" s="9" t="n">
-        <v>1.3125</v>
+      <c r="A37" s="8" t="n">
+        <v>41203</v>
+      </c>
+      <c r="B37" s="8" t="n">
+        <v>41203.3125</v>
       </c>
       <c r="C37" s="12" t="s">
         <v>36</v>
@@ -1737,17 +1749,19 @@
       <c r="G37" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="H37" s="9"/>
+      <c r="H37" s="9" t="n">
+        <v>2</v>
+      </c>
       <c r="I37" s="9" t="n">
         <v>1.3125</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="38">
-      <c r="A38" s="9" t="n">
-        <v>1.3125</v>
-      </c>
-      <c r="B38" s="9" t="n">
-        <v>1.33333333333333</v>
+      <c r="A38" s="8" t="n">
+        <v>41203.3125</v>
+      </c>
+      <c r="B38" s="8" t="n">
+        <v>41203.3333333333</v>
       </c>
       <c r="C38" s="12" t="s">
         <v>38</v>
@@ -1772,11 +1786,11 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="39">
-      <c r="A39" s="9" t="n">
-        <v>1.33333333333334</v>
-      </c>
-      <c r="B39" s="9" t="n">
-        <v>1.35416666666667</v>
+      <c r="A39" s="8" t="n">
+        <v>41203.3333333333</v>
+      </c>
+      <c r="B39" s="8" t="n">
+        <v>41203.3541666667</v>
       </c>
       <c r="C39" s="12" t="s">
         <v>38</v>
@@ -1801,11 +1815,11 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="40">
-      <c r="A40" s="9" t="n">
-        <v>1.35416666666667</v>
-      </c>
-      <c r="B40" s="9" t="n">
-        <v>1.375</v>
+      <c r="A40" s="8" t="n">
+        <v>41203.3541666667</v>
+      </c>
+      <c r="B40" s="8" t="n">
+        <v>41203.375</v>
       </c>
       <c r="C40" s="12" t="s">
         <v>39</v>
@@ -1830,11 +1844,11 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="41">
-      <c r="A41" s="9" t="n">
-        <v>1.375</v>
-      </c>
-      <c r="B41" s="9" t="n">
-        <v>1.39583333333333</v>
+      <c r="A41" s="8" t="n">
+        <v>41203.375</v>
+      </c>
+      <c r="B41" s="8" t="n">
+        <v>41203.3958333333</v>
       </c>
       <c r="C41" s="12" t="s">
         <v>40</v>
@@ -1859,11 +1873,11 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="42">
-      <c r="A42" s="9" t="n">
-        <v>1.39583333333333</v>
-      </c>
-      <c r="B42" s="9" t="n">
-        <v>1.41666666666667</v>
+      <c r="A42" s="8" t="n">
+        <v>41203.3958333333</v>
+      </c>
+      <c r="B42" s="8" t="n">
+        <v>41203.4166666667</v>
       </c>
       <c r="C42" s="12" t="s">
         <v>40</v>
@@ -1888,11 +1902,11 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="43">
-      <c r="A43" s="9" t="n">
-        <v>1.41666666666667</v>
-      </c>
-      <c r="B43" s="9" t="n">
-        <v>1.4375</v>
+      <c r="A43" s="8" t="n">
+        <v>41203.4166666667</v>
+      </c>
+      <c r="B43" s="8" t="n">
+        <v>41203.4375</v>
       </c>
       <c r="C43" s="12" t="s">
         <v>40</v>
@@ -1917,8 +1931,8 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="44">
-      <c r="A44" s="9"/>
-      <c r="B44" s="9"/>
+      <c r="A44" s="8"/>
+      <c r="B44" s="8"/>
       <c r="C44" s="7" t="s">
         <v>8</v>
       </c>
@@ -1938,11 +1952,11 @@
       <c r="I44" s="9"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14" outlineLevel="0" r="45">
-      <c r="A45" s="9" t="n">
-        <v>1.4375</v>
-      </c>
-      <c r="B45" s="9" t="n">
-        <v>1.45833333333334</v>
+      <c r="A45" s="8" t="n">
+        <v>41203.4375</v>
+      </c>
+      <c r="B45" s="8" t="n">
+        <v>41203.4583333333</v>
       </c>
       <c r="C45" s="7" t="s">
         <v>44</v>
@@ -1967,11 +1981,11 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="46">
-      <c r="A46" s="9" t="n">
-        <v>1.45833333333333</v>
-      </c>
-      <c r="B46" s="9" t="n">
-        <v>1.47916666666667</v>
+      <c r="A46" s="8" t="n">
+        <v>41203.4583333333</v>
+      </c>
+      <c r="B46" s="8" t="n">
+        <v>41203.4791666667</v>
       </c>
       <c r="C46" s="7" t="s">
         <v>48</v>
@@ -1994,11 +2008,11 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="47">
-      <c r="A47" s="9" t="n">
-        <v>1.47916666666667</v>
-      </c>
-      <c r="B47" s="9" t="n">
-        <v>1.5</v>
+      <c r="A47" s="8" t="n">
+        <v>41203.4791666667</v>
+      </c>
+      <c r="B47" s="8" t="n">
+        <v>41203.5</v>
       </c>
       <c r="C47" s="7" t="s">
         <v>45</v>
@@ -2023,11 +2037,11 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="48">
-      <c r="A48" s="9" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="B48" s="9" t="n">
-        <v>1.52083333333334</v>
+      <c r="A48" s="8" t="n">
+        <v>41203.5</v>
+      </c>
+      <c r="B48" s="8" t="n">
+        <v>41203.5208333333</v>
       </c>
       <c r="C48" s="15" t="s">
         <v>21</v>
@@ -2052,11 +2066,11 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="49">
-      <c r="A49" s="9" t="n">
-        <v>1.52083333333333</v>
-      </c>
-      <c r="B49" s="9" t="n">
-        <v>1.54166666666667</v>
+      <c r="A49" s="8" t="n">
+        <v>41203.5208333333</v>
+      </c>
+      <c r="B49" s="8" t="n">
+        <v>41203.5416666667</v>
       </c>
       <c r="C49" s="7" t="s">
         <v>47</v>
@@ -2081,11 +2095,11 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14" outlineLevel="0" r="50">
-      <c r="A50" s="9" t="n">
-        <v>1.54166666666667</v>
-      </c>
-      <c r="B50" s="9" t="n">
-        <v>1.5625</v>
+      <c r="A50" s="8" t="n">
+        <v>41203.5416666667</v>
+      </c>
+      <c r="B50" s="8" t="n">
+        <v>41203.5625</v>
       </c>
       <c r="C50" s="7" t="s">
         <v>49</v>
@@ -2110,11 +2124,11 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="51">
-      <c r="A51" s="9" t="n">
-        <v>1.5625</v>
-      </c>
-      <c r="B51" s="9" t="n">
-        <v>1.58333333333334</v>
+      <c r="A51" s="8" t="n">
+        <v>41203.5625</v>
+      </c>
+      <c r="B51" s="8" t="n">
+        <v>41203.5833333333</v>
       </c>
       <c r="C51" s="7" t="s">
         <v>51</v>
@@ -2137,11 +2151,11 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="52">
-      <c r="A52" s="9" t="n">
-        <v>1.58333333333333</v>
-      </c>
-      <c r="B52" s="9" t="n">
-        <v>1.60416666666667</v>
+      <c r="A52" s="8" t="n">
+        <v>41203.5833333333</v>
+      </c>
+      <c r="B52" s="8" t="n">
+        <v>41203.6041666667</v>
       </c>
       <c r="C52" s="12" t="s">
         <v>53</v>
@@ -2166,11 +2180,11 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="53">
-      <c r="A53" s="9" t="n">
-        <v>1.60416666666667</v>
-      </c>
-      <c r="B53" s="9" t="n">
-        <v>0.635416666666667</v>
+      <c r="A53" s="8" t="n">
+        <v>41203.6041666667</v>
+      </c>
+      <c r="B53" s="8" t="n">
+        <v>41203.6354166667</v>
       </c>
       <c r="C53" s="12" t="s">
         <v>53</v>
@@ -2195,11 +2209,11 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="54">
-      <c r="A54" s="9" t="n">
-        <v>0.635416666666667</v>
-      </c>
-      <c r="B54" s="9" t="n">
-        <v>0.645833333333333</v>
+      <c r="A54" s="8" t="n">
+        <v>41203.6354166667</v>
+      </c>
+      <c r="B54" s="8" t="n">
+        <v>41203.6458333333</v>
       </c>
       <c r="C54" s="12" t="s">
         <v>54</v>
@@ -2249,7 +2263,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="landscape" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2269,13 +2283,14 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="7.02745098039216"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="9.18039215686274"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.3294117647059"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="13.0509803921569"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="11.4745098039216"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="20.0862745098039"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="9.18039215686274"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="7.08627450980392"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="9.25882352941177"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.4235294117647"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="13.1647058823529"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="11.5725490196078"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="20.2588235294118"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="9.25882352941177"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.57647058823529"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="20" outlineLevel="0" r="1">
@@ -2450,13 +2465,13 @@
       <c r="E9" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="F9" s="20" t="s">
+      <c r="F9" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="G9" s="20" t="s">
+      <c r="G9" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="H9" s="20" t="s">
+      <c r="H9" s="19" t="s">
         <v>43</v>
       </c>
     </row>
@@ -2860,7 +2875,7 @@
       <c r="C25" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="D25" s="21" t="s">
+      <c r="D25" s="20" t="s">
         <v>76</v>
       </c>
       <c r="E25" s="19" t="s">
@@ -2892,7 +2907,7 @@
       <c r="C26" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="D26" s="21"/>
+      <c r="D26" s="20"/>
       <c r="E26" s="19" t="s">
         <v>75</v>
       </c>
@@ -2920,7 +2935,7 @@
       <c r="C27" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="D27" s="21" t="s">
+      <c r="D27" s="20" t="s">
         <v>81</v>
       </c>
       <c r="E27" s="19" t="s">
@@ -2950,7 +2965,7 @@
       <c r="C28" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="D28" s="21"/>
+      <c r="D28" s="20"/>
       <c r="E28" s="19" t="s">
         <v>79</v>
       </c>
@@ -2978,7 +2993,7 @@
       <c r="C29" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="D29" s="21" t="s">
+      <c r="D29" s="20" t="s">
         <v>84</v>
       </c>
       <c r="E29" s="19" t="s">
@@ -3008,7 +3023,7 @@
       <c r="C30" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="D30" s="21"/>
+      <c r="D30" s="20"/>
       <c r="E30" s="19" t="s">
         <v>83</v>
       </c>
@@ -3129,16 +3144,16 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="20" outlineLevel="0" r="36">
-      <c r="A36" s="22"/>
-      <c r="B36" s="22"/>
-      <c r="C36" s="23" t="s">
+      <c r="A36" s="21"/>
+      <c r="B36" s="21"/>
+      <c r="C36" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="D36" s="23"/>
-      <c r="E36" s="23"/>
-      <c r="F36" s="23"/>
-      <c r="G36" s="23"/>
-      <c r="H36" s="24"/>
+      <c r="D36" s="22"/>
+      <c r="E36" s="22"/>
+      <c r="F36" s="22"/>
+      <c r="G36" s="22"/>
+      <c r="H36" s="23"/>
       <c r="I36" s="4"/>
       <c r="J36" s="4"/>
     </row>
@@ -3461,11 +3476,11 @@
       <c r="B51" s="18" t="n">
         <v>1.52083333333334</v>
       </c>
-      <c r="C51" s="21" t="s">
+      <c r="C51" s="20" t="s">
         <v>105</v>
       </c>
       <c r="D51" s="11"/>
-      <c r="E51" s="21" t="s">
+      <c r="E51" s="20" t="s">
         <v>103</v>
       </c>
       <c r="F51" s="11"/>
@@ -3674,7 +3689,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="landscape" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
Sterted to fix Groot as well, needs debugging though
</commit_message>
<xml_diff>
--- a/data/planning_2012_edit.xlsx
+++ b/data/planning_2012_edit.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="116">
   <si>
     <t>Kleine speltakken</t>
   </si>
@@ -370,10 +370,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
     <numFmt formatCode="DD/MM/YY\ HH:MM" numFmtId="165"/>
     <numFmt formatCode="H:MM" numFmtId="166"/>
+    <numFmt formatCode="DD/MM/YYYY\ HH:MM" numFmtId="167"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -496,7 +497,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
@@ -549,10 +550,19 @@
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="0" fontId="5" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="false" borderId="2" fillId="0" fontId="0" numFmtId="167" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="false" borderId="3" fillId="0" fontId="0" numFmtId="167" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+    </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="false" borderId="3" fillId="0" fontId="0" numFmtId="166" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="0" fontId="0" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="167" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="0" fontId="0" numFmtId="164" xfId="0">
@@ -591,14 +601,14 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="13.7019607843137"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="2" width="10.6980392156863"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="17.7843137254902"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="11.7176470588235"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="12.2901960784314"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="9.25882352941177"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="8.53333333333333"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.57647058823529"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="13.7529411764706"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="2" width="10.7411764705882"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="17.8627450980392"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="11.7686274509804"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="12.3411764705882"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="9.30196078431373"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="8.56862745098039"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.61176470588235"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="20" outlineLevel="0" r="1">
@@ -2283,14 +2293,14 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="7.08627450980392"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="9.25882352941177"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.4235294117647"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="13.1647058823529"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="11.5725490196078"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="20.2588235294118"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="9.25882352941177"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.57647058823529"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="15.7843137254902"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="9.30196078431373"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.4745098039216"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="13.2235294117647"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="11.6156862745098"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="20.3450980392157"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="9.30196078431373"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.61176470588235"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="20" outlineLevel="0" r="1">
@@ -2330,157 +2340,225 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="3">
-      <c r="A3" s="9" t="n">
-        <v>0.395833333333333</v>
-      </c>
-      <c r="B3" s="18" t="n">
-        <v>0.416666666666667</v>
-      </c>
-      <c r="C3" s="19" t="s">
+      <c r="A3" s="18" t="n">
+        <v>41202.3958333333</v>
+      </c>
+      <c r="B3" s="19" t="n">
+        <v>41202.4166666667</v>
+      </c>
+      <c r="C3" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
+      <c r="D3" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="20" t="s">
+        <v>11</v>
+      </c>
       <c r="I3" s="9" t="n">
         <v>0.395833333333333</v>
       </c>
-      <c r="J3" s="18" t="n">
+      <c r="J3" s="21" t="n">
         <v>0.416666666666667</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="4">
-      <c r="A4" s="9" t="n">
-        <v>0.416666666666667</v>
-      </c>
-      <c r="B4" s="18" t="n">
-        <v>0.4375</v>
+      <c r="A4" s="18" t="n">
+        <v>41202.4166666667</v>
+      </c>
+      <c r="B4" s="19" t="n">
+        <v>41202.4375</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
+      <c r="D4" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>56</v>
+      </c>
       <c r="I4" s="9" t="n">
         <v>0.416666666666667</v>
       </c>
-      <c r="J4" s="18" t="n">
+      <c r="J4" s="21" t="n">
         <v>0.4375</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="5">
-      <c r="A5" s="9" t="n">
-        <v>0.4375</v>
-      </c>
-      <c r="B5" s="18" t="n">
-        <v>0.458333333333333</v>
-      </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
+      <c r="A5" s="18" t="n">
+        <v>41202.4375</v>
+      </c>
+      <c r="B5" s="19" t="n">
+        <v>41202.4583333333</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>56</v>
+      </c>
       <c r="I5" s="9" t="n">
         <v>0.4375</v>
       </c>
-      <c r="J5" s="18" t="n">
+      <c r="J5" s="21" t="n">
         <v>0.458333333333333</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="6">
-      <c r="A6" s="9" t="n">
-        <v>0.458333333333333</v>
-      </c>
-      <c r="B6" s="18" t="n">
-        <v>0.479166666666667</v>
-      </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
+      <c r="A6" s="18" t="n">
+        <v>41202.4583333333</v>
+      </c>
+      <c r="B6" s="19" t="n">
+        <v>41202.4791666667</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>56</v>
+      </c>
       <c r="I6" s="9" t="n">
         <v>0.458333333333333</v>
       </c>
-      <c r="J6" s="18" t="n">
+      <c r="J6" s="21" t="n">
         <v>0.479166666666667</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="7">
-      <c r="A7" s="9" t="n">
-        <v>0.479166666666667</v>
-      </c>
-      <c r="B7" s="18" t="n">
-        <v>0.5</v>
+      <c r="A7" s="18" t="n">
+        <v>41202.4791666667</v>
+      </c>
+      <c r="B7" s="19" t="n">
+        <v>41202.5</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
+      <c r="D7" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>57</v>
+      </c>
       <c r="I7" s="9" t="n">
         <v>0.479166666666667</v>
       </c>
-      <c r="J7" s="18" t="n">
+      <c r="J7" s="21" t="n">
         <v>0.5</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="8">
-      <c r="A8" s="9" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="B8" s="18" t="n">
-        <v>0.520833333333334</v>
-      </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
+      <c r="A8" s="18" t="n">
+        <v>41202.5</v>
+      </c>
+      <c r="B8" s="19" t="n">
+        <v>41202.5208333333</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>57</v>
+      </c>
       <c r="I8" s="9" t="n">
         <v>0.5</v>
       </c>
-      <c r="J8" s="18" t="n">
+      <c r="J8" s="21" t="n">
         <v>0.520833333333334</v>
       </c>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="9" s="1">
-      <c r="C9" s="19" t="s">
+      <c r="A9" s="22"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="19" t="s">
+      <c r="D9" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="19" t="s">
+      <c r="E9" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="F9" s="19" t="s">
+      <c r="F9" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="G9" s="19" t="s">
+      <c r="G9" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="H9" s="19" t="s">
+      <c r="H9" s="20" t="s">
         <v>43</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="10">
-      <c r="A10" s="9" t="n">
-        <v>0.520833333333333</v>
-      </c>
-      <c r="B10" s="18" t="n">
-        <v>0.541666666666667</v>
+      <c r="A10" s="18" t="n">
+        <v>41202.5208333333</v>
+      </c>
+      <c r="B10" s="19" t="n">
+        <v>41202.5416666667</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>61</v>
@@ -2503,16 +2581,16 @@
       <c r="I10" s="9" t="n">
         <v>0.520833333333333</v>
       </c>
-      <c r="J10" s="18" t="n">
+      <c r="J10" s="21" t="n">
         <v>0.541666666666667</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="11">
-      <c r="A11" s="9" t="n">
-        <v>0.541666666666667</v>
-      </c>
-      <c r="B11" s="18" t="n">
-        <v>0.5625</v>
+      <c r="A11" s="18" t="n">
+        <v>41202.5416666667</v>
+      </c>
+      <c r="B11" s="19" t="n">
+        <v>41202.5625</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>64</v>
@@ -2531,16 +2609,16 @@
       <c r="I11" s="9" t="n">
         <v>0.541666666666667</v>
       </c>
-      <c r="J11" s="18" t="n">
+      <c r="J11" s="21" t="n">
         <v>0.5625</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14" outlineLevel="0" r="12">
-      <c r="A12" s="9" t="n">
-        <v>0.5625</v>
-      </c>
-      <c r="B12" s="18" t="n">
-        <v>0.583333333333334</v>
+      <c r="A12" s="18" t="n">
+        <v>41202.5625</v>
+      </c>
+      <c r="B12" s="19" t="n">
+        <v>41202.5833333333</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>67</v>
@@ -2563,16 +2641,16 @@
       <c r="I12" s="9" t="n">
         <v>0.5625</v>
       </c>
-      <c r="J12" s="18" t="n">
+      <c r="J12" s="21" t="n">
         <v>0.583333333333334</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="13">
-      <c r="A13" s="9" t="n">
-        <v>0.583333333333333</v>
-      </c>
-      <c r="B13" s="18" t="n">
-        <v>0.604166666666667</v>
+      <c r="A13" s="18" t="n">
+        <v>41202.5833333333</v>
+      </c>
+      <c r="B13" s="19" t="n">
+        <v>41202.6041666667</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>70</v>
@@ -2591,16 +2669,16 @@
       <c r="I13" s="9" t="n">
         <v>0.583333333333333</v>
       </c>
-      <c r="J13" s="18" t="n">
+      <c r="J13" s="21" t="n">
         <v>0.604166666666667</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="14">
-      <c r="A14" s="9" t="n">
-        <v>0.604166666666667</v>
-      </c>
-      <c r="B14" s="18" t="n">
-        <v>0.625</v>
+      <c r="A14" s="18" t="n">
+        <v>41202.6041666667</v>
+      </c>
+      <c r="B14" s="19" t="n">
+        <v>41202.625</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>72</v>
@@ -2623,16 +2701,16 @@
       <c r="I14" s="9" t="n">
         <v>0.604166666666667</v>
       </c>
-      <c r="J14" s="18" t="n">
+      <c r="J14" s="21" t="n">
         <v>0.625</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="15">
-      <c r="A15" s="9" t="n">
-        <v>0.625</v>
-      </c>
-      <c r="B15" s="18" t="n">
-        <v>0.645833333333333</v>
+      <c r="A15" s="18" t="n">
+        <v>41202.625</v>
+      </c>
+      <c r="B15" s="19" t="n">
+        <v>41202.6458333333</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>62</v>
@@ -2651,16 +2729,16 @@
       <c r="I15" s="9" t="n">
         <v>0.625</v>
       </c>
-      <c r="J15" s="18" t="n">
+      <c r="J15" s="21" t="n">
         <v>0.645833333333333</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14" outlineLevel="0" r="16">
-      <c r="A16" s="9" t="n">
-        <v>0.645833333333333</v>
-      </c>
-      <c r="B16" s="18" t="n">
-        <v>0.666666666666667</v>
+      <c r="A16" s="18" t="n">
+        <v>41202.6458333333</v>
+      </c>
+      <c r="B16" s="19" t="n">
+        <v>41202.6666666667</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>66</v>
@@ -2683,16 +2761,16 @@
       <c r="I16" s="9" t="n">
         <v>0.645833333333333</v>
       </c>
-      <c r="J16" s="18" t="n">
+      <c r="J16" s="21" t="n">
         <v>0.666666666666667</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="17">
-      <c r="A17" s="9" t="n">
-        <v>0.666666666666667</v>
-      </c>
-      <c r="B17" s="18" t="n">
-        <v>0.6875</v>
+      <c r="A17" s="18" t="n">
+        <v>41202.6666666667</v>
+      </c>
+      <c r="B17" s="19" t="n">
+        <v>41202.6875</v>
       </c>
       <c r="C17" s="7" t="s">
         <v>68</v>
@@ -2711,180 +2789,246 @@
       <c r="I17" s="9" t="n">
         <v>0.666666666666667</v>
       </c>
-      <c r="J17" s="18" t="n">
+      <c r="J17" s="21" t="n">
         <v>0.6875</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="18">
-      <c r="A18" s="9" t="n">
-        <v>0.6875</v>
-      </c>
-      <c r="B18" s="18" t="n">
-        <v>0.708333333333333</v>
+      <c r="A18" s="18" t="n">
+        <v>41202.6875</v>
+      </c>
+      <c r="B18" s="19" t="n">
+        <v>41202.7083333333</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
+      <c r="D18" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="H18" s="7" t="s">
+        <v>57</v>
+      </c>
       <c r="I18" s="9" t="n">
         <v>0.6875</v>
       </c>
-      <c r="J18" s="18" t="n">
+      <c r="J18" s="21" t="n">
         <v>0.708333333333333</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="19">
-      <c r="A19" s="9" t="n">
-        <v>0.708333333333334</v>
-      </c>
-      <c r="B19" s="18" t="n">
-        <v>0.729166666666667</v>
-      </c>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
+      <c r="A19" s="18" t="n">
+        <v>41202.7083333333</v>
+      </c>
+      <c r="B19" s="19" t="n">
+        <v>41202.7291666667</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="H19" s="7" t="s">
+        <v>57</v>
+      </c>
       <c r="I19" s="9" t="n">
         <v>0.708333333333334</v>
       </c>
-      <c r="J19" s="18" t="n">
+      <c r="J19" s="21" t="n">
         <v>0.729166666666667</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="20">
-      <c r="A20" s="9" t="n">
-        <v>0.729166666666667</v>
-      </c>
-      <c r="B20" s="18" t="n">
-        <v>0.75</v>
+      <c r="A20" s="18" t="n">
+        <v>41202.7291666667</v>
+      </c>
+      <c r="B20" s="19" t="n">
+        <v>41202.75</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
+      <c r="D20" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="H20" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="I20" s="9" t="n">
         <v>0.729166666666667</v>
       </c>
-      <c r="J20" s="18" t="n">
+      <c r="J20" s="21" t="n">
         <v>0.75</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="21">
-      <c r="A21" s="9" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="B21" s="18" t="n">
-        <v>0.770833333333333</v>
-      </c>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
+      <c r="A21" s="18" t="n">
+        <v>41202.75</v>
+      </c>
+      <c r="B21" s="19" t="n">
+        <v>41202.7708333333</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="H21" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="I21" s="9" t="n">
         <v>0.75</v>
       </c>
-      <c r="J21" s="18" t="n">
+      <c r="J21" s="21" t="n">
         <v>0.770833333333333</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="22">
-      <c r="A22" s="9" t="n">
-        <v>0.770833333333334</v>
-      </c>
-      <c r="B22" s="18" t="n">
-        <v>0.791666666666667</v>
+      <c r="A22" s="18" t="n">
+        <v>41202.7708333333</v>
+      </c>
+      <c r="B22" s="19" t="n">
+        <v>41202.7916666667</v>
       </c>
       <c r="C22" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
+      <c r="D22" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="H22" s="7" t="s">
+        <v>32</v>
+      </c>
       <c r="I22" s="9" t="n">
         <v>0.770833333333334</v>
       </c>
-      <c r="J22" s="18" t="n">
+      <c r="J22" s="21" t="n">
         <v>0.791666666666667</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="23">
-      <c r="A23" s="9" t="n">
-        <v>0.791666666666667</v>
-      </c>
-      <c r="B23" s="18" t="n">
-        <v>0.8125</v>
-      </c>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
+      <c r="A23" s="18" t="n">
+        <v>41202.7916666667</v>
+      </c>
+      <c r="B23" s="19" t="n">
+        <v>41202.8125</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="H23" s="7" t="s">
+        <v>32</v>
+      </c>
       <c r="I23" s="9" t="n">
         <v>0.791666666666667</v>
       </c>
-      <c r="J23" s="18" t="n">
+      <c r="J23" s="21" t="n">
         <v>0.8125</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="24">
-      <c r="A24" s="9"/>
-      <c r="B24" s="18"/>
-      <c r="C24" s="19" t="s">
+      <c r="A24" s="18"/>
+      <c r="B24" s="19"/>
+      <c r="C24" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="D24" s="19" t="s">
+      <c r="D24" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="E24" s="19" t="s">
+      <c r="E24" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="F24" s="19" t="s">
+      <c r="F24" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="G24" s="19" t="s">
+      <c r="G24" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="H24" s="19" t="s">
+      <c r="H24" s="20" t="s">
         <v>74</v>
       </c>
       <c r="I24" s="9"/>
-      <c r="J24" s="18"/>
+      <c r="J24" s="21"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14" outlineLevel="0" r="25">
-      <c r="A25" s="9" t="n">
-        <v>0.8125</v>
-      </c>
-      <c r="B25" s="18" t="n">
-        <v>0.826388888888889</v>
-      </c>
-      <c r="C25" s="19" t="s">
+      <c r="A25" s="18" t="n">
+        <v>41202.8125</v>
+      </c>
+      <c r="B25" s="19" t="n">
+        <v>41202.8263888889</v>
+      </c>
+      <c r="C25" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="D25" s="20" t="s">
+      <c r="D25" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="E25" s="19" t="s">
+      <c r="E25" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="F25" s="19" t="s">
+      <c r="F25" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="G25" s="19" t="s">
+      <c r="G25" s="20" t="s">
         <v>79</v>
       </c>
       <c r="H25" s="11" t="s">
@@ -2893,267 +3037,325 @@
       <c r="I25" s="9" t="n">
         <v>0.8125</v>
       </c>
-      <c r="J25" s="18" t="n">
+      <c r="J25" s="21" t="n">
         <v>0.826388888888889</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="26">
-      <c r="A26" s="9" t="n">
-        <v>0.826388888888889</v>
-      </c>
-      <c r="B26" s="18" t="n">
-        <v>0.840277777777778</v>
-      </c>
-      <c r="C26" s="19" t="s">
+      <c r="A26" s="18" t="n">
+        <v>41202.8263888889</v>
+      </c>
+      <c r="B26" s="19" t="n">
+        <v>41202.8402777778</v>
+      </c>
+      <c r="C26" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="D26" s="20"/>
-      <c r="E26" s="19" t="s">
+      <c r="D26" s="23"/>
+      <c r="E26" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="F26" s="19" t="s">
+      <c r="F26" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="G26" s="19" t="s">
+      <c r="G26" s="20" t="s">
         <v>78</v>
       </c>
       <c r="H26" s="11"/>
       <c r="I26" s="9" t="n">
         <v>0.826388888888889</v>
       </c>
-      <c r="J26" s="18" t="n">
+      <c r="J26" s="21" t="n">
         <v>0.840277777777778</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14" outlineLevel="0" r="27">
-      <c r="A27" s="9" t="n">
-        <v>0.840277777777778</v>
-      </c>
-      <c r="B27" s="18" t="n">
-        <v>0.854166666666667</v>
-      </c>
-      <c r="C27" s="19" t="s">
+      <c r="A27" s="18" t="n">
+        <v>41202.8402777778</v>
+      </c>
+      <c r="B27" s="19" t="n">
+        <v>41202.8541666667</v>
+      </c>
+      <c r="C27" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="D27" s="20" t="s">
+      <c r="D27" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="E27" s="19" t="s">
+      <c r="E27" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="F27" s="19" t="s">
+      <c r="F27" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="G27" s="19" t="s">
+      <c r="G27" s="20" t="s">
         <v>83</v>
       </c>
       <c r="H27" s="11"/>
       <c r="I27" s="9" t="n">
         <v>0.840277777777778</v>
       </c>
-      <c r="J27" s="18" t="n">
+      <c r="J27" s="21" t="n">
         <v>0.854166666666667</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="28">
-      <c r="A28" s="9" t="n">
-        <v>0.854166666666667</v>
-      </c>
-      <c r="B28" s="18" t="n">
-        <v>0.868055555555556</v>
-      </c>
-      <c r="C28" s="19" t="s">
+      <c r="A28" s="18" t="n">
+        <v>41202.8541666667</v>
+      </c>
+      <c r="B28" s="19" t="n">
+        <v>41202.8680555556</v>
+      </c>
+      <c r="C28" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="D28" s="20"/>
-      <c r="E28" s="19" t="s">
+      <c r="D28" s="23"/>
+      <c r="E28" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="F28" s="19" t="s">
+      <c r="F28" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="G28" s="19" t="s">
+      <c r="G28" s="20" t="s">
         <v>82</v>
       </c>
       <c r="H28" s="11"/>
       <c r="I28" s="9" t="n">
         <v>0.854166666666667</v>
       </c>
-      <c r="J28" s="18" t="n">
+      <c r="J28" s="21" t="n">
         <v>0.868055555555556</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14" outlineLevel="0" r="29">
-      <c r="A29" s="9" t="n">
-        <v>0.868055555555556</v>
-      </c>
-      <c r="B29" s="18" t="n">
-        <v>0.881944444444444</v>
-      </c>
-      <c r="C29" s="19" t="s">
+      <c r="A29" s="18" t="n">
+        <v>41202.8680555556</v>
+      </c>
+      <c r="B29" s="19" t="n">
+        <v>41202.8819444445</v>
+      </c>
+      <c r="C29" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="D29" s="20" t="s">
+      <c r="D29" s="23" t="s">
         <v>84</v>
       </c>
-      <c r="E29" s="19" t="s">
+      <c r="E29" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="F29" s="19" t="s">
+      <c r="F29" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="G29" s="19" t="s">
+      <c r="G29" s="20" t="s">
         <v>75</v>
       </c>
       <c r="H29" s="11"/>
       <c r="I29" s="9" t="n">
         <v>0.868055555555556</v>
       </c>
-      <c r="J29" s="18" t="n">
+      <c r="J29" s="21" t="n">
         <v>0.881944444444444</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="30">
-      <c r="A30" s="9" t="n">
-        <v>0.881944444444444</v>
-      </c>
-      <c r="B30" s="18" t="n">
-        <v>0.895833333333333</v>
-      </c>
-      <c r="C30" s="19" t="s">
+      <c r="A30" s="18" t="n">
+        <v>41202.8819444445</v>
+      </c>
+      <c r="B30" s="19" t="n">
+        <v>41202.8958333333</v>
+      </c>
+      <c r="C30" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="D30" s="20"/>
-      <c r="E30" s="19" t="s">
+      <c r="D30" s="23"/>
+      <c r="E30" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="F30" s="19" t="s">
+      <c r="F30" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="G30" s="19" t="s">
+      <c r="G30" s="20" t="s">
         <v>77</v>
       </c>
       <c r="H30" s="11"/>
       <c r="I30" s="9" t="n">
         <v>0.881944444444444</v>
       </c>
-      <c r="J30" s="18" t="n">
+      <c r="J30" s="21" t="n">
         <v>0.895833333333333</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="31">
-      <c r="A31" s="9" t="n">
-        <v>0.895833333333334</v>
-      </c>
-      <c r="B31" s="18" t="n">
-        <v>0.916666666666667</v>
+      <c r="A31" s="18" t="n">
+        <v>41202.8958333333</v>
+      </c>
+      <c r="B31" s="19" t="n">
+        <v>41202.9166666667</v>
       </c>
       <c r="C31" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="7"/>
-      <c r="H31" s="7"/>
+      <c r="D31" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="F31" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="G31" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="H31" s="7" t="s">
+        <v>85</v>
+      </c>
       <c r="I31" s="9" t="n">
         <v>0.895833333333334</v>
       </c>
-      <c r="J31" s="18" t="n">
+      <c r="J31" s="21" t="n">
         <v>0.916666666666667</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="32">
-      <c r="A32" s="9" t="n">
-        <v>0.916666666666667</v>
-      </c>
-      <c r="B32" s="18" t="n">
-        <v>0.9375</v>
-      </c>
-      <c r="C32" s="7"/>
-      <c r="D32" s="7"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
-      <c r="G32" s="7"/>
-      <c r="H32" s="7"/>
+      <c r="A32" s="18" t="n">
+        <v>41202.9166666667</v>
+      </c>
+      <c r="B32" s="19" t="n">
+        <v>41202.9375</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="F32" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="G32" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="H32" s="7" t="s">
+        <v>85</v>
+      </c>
       <c r="I32" s="9" t="n">
         <v>0.916666666666667</v>
       </c>
-      <c r="J32" s="18" t="n">
+      <c r="J32" s="21" t="n">
         <v>0.9375</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="33">
-      <c r="A33" s="9" t="n">
-        <v>0.937500000000001</v>
-      </c>
-      <c r="B33" s="18" t="n">
-        <v>0.958333333333333</v>
-      </c>
-      <c r="C33" s="7"/>
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
-      <c r="G33" s="7"/>
-      <c r="H33" s="7"/>
+      <c r="A33" s="18" t="n">
+        <v>41202.9375</v>
+      </c>
+      <c r="B33" s="19" t="n">
+        <v>41202.9583333333</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="F33" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="G33" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="H33" s="7" t="s">
+        <v>85</v>
+      </c>
       <c r="I33" s="9" t="n">
         <v>0.937500000000001</v>
       </c>
-      <c r="J33" s="18" t="n">
+      <c r="J33" s="21" t="n">
         <v>0.958333333333333</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="34">
-      <c r="A34" s="9" t="n">
-        <v>0.958333333333334</v>
-      </c>
-      <c r="B34" s="18" t="n">
-        <v>0.979166666666667</v>
-      </c>
-      <c r="C34" s="7"/>
-      <c r="D34" s="7"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="7"/>
-      <c r="G34" s="7"/>
-      <c r="H34" s="7"/>
+      <c r="A34" s="18" t="n">
+        <v>41202.9583333333</v>
+      </c>
+      <c r="B34" s="19" t="n">
+        <v>41202.9791666667</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="F34" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="G34" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="H34" s="7" t="s">
+        <v>85</v>
+      </c>
       <c r="I34" s="9" t="n">
         <v>0.958333333333334</v>
       </c>
-      <c r="J34" s="18" t="n">
+      <c r="J34" s="21" t="n">
         <v>0.979166666666667</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="35">
-      <c r="A35" s="9" t="n">
-        <v>0.979166666666667</v>
-      </c>
-      <c r="B35" s="18" t="n">
+      <c r="A35" s="18" t="n">
+        <v>41202.9791666667</v>
+      </c>
+      <c r="B35" s="19" t="n">
         <v>1</v>
       </c>
-      <c r="C35" s="7"/>
-      <c r="D35" s="7"/>
-      <c r="E35" s="7"/>
-      <c r="F35" s="7"/>
-      <c r="G35" s="7"/>
-      <c r="H35" s="7"/>
+      <c r="C35" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="F35" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="G35" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="H35" s="7" t="s">
+        <v>85</v>
+      </c>
       <c r="I35" s="9" t="n">
         <v>0.979166666666667</v>
       </c>
-      <c r="J35" s="18" t="n">
+      <c r="J35" s="21" t="n">
         <v>1</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="20" outlineLevel="0" r="36">
-      <c r="A36" s="21"/>
-      <c r="B36" s="21"/>
-      <c r="C36" s="22" t="s">
+      <c r="A36" s="24"/>
+      <c r="B36" s="24"/>
+      <c r="C36" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="D36" s="22"/>
-      <c r="E36" s="22"/>
-      <c r="F36" s="22"/>
-      <c r="G36" s="22"/>
-      <c r="H36" s="23"/>
+      <c r="D36" s="25"/>
+      <c r="E36" s="25"/>
+      <c r="F36" s="25"/>
+      <c r="G36" s="25"/>
+      <c r="H36" s="26"/>
       <c r="I36" s="4"/>
       <c r="J36" s="4"/>
     </row>
@@ -3179,93 +3381,149 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="38">
-      <c r="A38" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="B38" s="18"/>
+      <c r="A38" s="18" t="n">
+        <v>41203</v>
+      </c>
+      <c r="B38" s="19" t="n">
+        <v>41201.3125</v>
+      </c>
       <c r="C38" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D38" s="7"/>
-      <c r="E38" s="7"/>
-      <c r="F38" s="7"/>
-      <c r="G38" s="7"/>
+      <c r="D38" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E38" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F38" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G38" s="7" t="s">
+        <v>36</v>
+      </c>
       <c r="H38" s="9" t="n">
         <v>0</v>
       </c>
-      <c r="I38" s="18"/>
+      <c r="I38" s="21"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="39">
-      <c r="A39" s="9"/>
-      <c r="B39" s="18"/>
-      <c r="C39" s="7"/>
-      <c r="D39" s="7"/>
-      <c r="E39" s="7"/>
-      <c r="F39" s="7"/>
-      <c r="G39" s="7"/>
+      <c r="A39" s="18" t="n">
+        <v>41204</v>
+      </c>
+      <c r="B39" s="19" t="n">
+        <v>41202.3125</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E39" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F39" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G39" s="7" t="s">
+        <v>36</v>
+      </c>
       <c r="H39" s="9"/>
-      <c r="I39" s="18"/>
+      <c r="I39" s="21"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="40">
-      <c r="A40" s="9"/>
-      <c r="B40" s="18" t="n">
+      <c r="A40" s="18" t="n">
+        <v>41205</v>
+      </c>
+      <c r="B40" s="19" t="n">
+        <v>41203.3125</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F40" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G40" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="H40" s="9"/>
+      <c r="I40" s="21" t="n">
         <v>1.3125</v>
       </c>
-      <c r="C40" s="7"/>
-      <c r="D40" s="7"/>
-      <c r="E40" s="7"/>
-      <c r="F40" s="7"/>
-      <c r="G40" s="7"/>
-      <c r="H40" s="9"/>
-      <c r="I40" s="18" t="n">
-        <v>1.3125</v>
-      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="41">
-      <c r="A41" s="9" t="n">
-        <v>1.3125</v>
-      </c>
-      <c r="B41" s="18" t="n">
-        <v>1.33333333333333</v>
+      <c r="A41" s="18" t="n">
+        <v>41203.3125</v>
+      </c>
+      <c r="B41" s="19" t="n">
+        <v>41203.3333333333</v>
       </c>
       <c r="C41" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="D41" s="7"/>
-      <c r="E41" s="7"/>
-      <c r="F41" s="7"/>
-      <c r="G41" s="7"/>
+      <c r="D41" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="F41" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="G41" s="7" t="s">
+        <v>86</v>
+      </c>
       <c r="H41" s="9" t="n">
         <v>1.3125</v>
       </c>
-      <c r="I41" s="18" t="n">
+      <c r="I41" s="21" t="n">
         <v>1.33333333333333</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="42">
-      <c r="A42" s="9" t="n">
-        <v>1.33333333333334</v>
-      </c>
-      <c r="B42" s="18" t="n">
-        <v>1.35416666666667</v>
+      <c r="A42" s="18" t="n">
+        <v>41203.3333333333</v>
+      </c>
+      <c r="B42" s="19" t="n">
+        <v>41203.3541666667</v>
       </c>
       <c r="C42" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D42" s="7"/>
-      <c r="E42" s="7"/>
-      <c r="F42" s="7"/>
-      <c r="G42" s="7"/>
+      <c r="D42" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E42" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F42" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G42" s="7" t="s">
+        <v>39</v>
+      </c>
       <c r="H42" s="9" t="n">
         <v>1.33333333333334</v>
       </c>
-      <c r="I42" s="18" t="n">
+      <c r="I42" s="21" t="n">
         <v>1.35416666666667</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="43">
-      <c r="A43" s="9"/>
-      <c r="B43" s="18"/>
+      <c r="A43" s="18" t="n">
+        <v>41202.3541666667</v>
+      </c>
+      <c r="B43" s="19" t="n">
+        <v>41202.375</v>
+      </c>
       <c r="C43" s="7" t="s">
         <v>4</v>
       </c>
@@ -3282,14 +3540,14 @@
         <v>87</v>
       </c>
       <c r="H43" s="9"/>
-      <c r="I43" s="18"/>
+      <c r="I43" s="21"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="44">
-      <c r="A44" s="9" t="n">
-        <v>1.35416666666667</v>
-      </c>
-      <c r="B44" s="18" t="n">
-        <v>1.375</v>
+      <c r="A44" s="18" t="n">
+        <v>41203.3541666667</v>
+      </c>
+      <c r="B44" s="19" t="n">
+        <v>41203.375</v>
       </c>
       <c r="C44" s="11" t="s">
         <v>88</v>
@@ -3309,16 +3567,16 @@
       <c r="H44" s="9" t="n">
         <v>1.35416666666667</v>
       </c>
-      <c r="I44" s="18" t="n">
+      <c r="I44" s="21" t="n">
         <v>1.375</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="45">
-      <c r="A45" s="9" t="n">
-        <v>1.375</v>
-      </c>
-      <c r="B45" s="18" t="n">
-        <v>1.39583333333333</v>
+      <c r="A45" s="18" t="n">
+        <v>41203.375</v>
+      </c>
+      <c r="B45" s="19" t="n">
+        <v>41203.3958333333</v>
       </c>
       <c r="C45" s="11" t="s">
         <v>90</v>
@@ -3332,16 +3590,16 @@
       <c r="H45" s="9" t="n">
         <v>1.375</v>
       </c>
-      <c r="I45" s="18" t="n">
+      <c r="I45" s="21" t="n">
         <v>1.39583333333333</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="46">
-      <c r="A46" s="9" t="n">
-        <v>1.39583333333333</v>
-      </c>
-      <c r="B46" s="18" t="n">
-        <v>1.41666666666667</v>
+      <c r="A46" s="18" t="n">
+        <v>41203.3958333333</v>
+      </c>
+      <c r="B46" s="19" t="n">
+        <v>41203.4166666667</v>
       </c>
       <c r="C46" s="11" t="s">
         <v>93</v>
@@ -3361,16 +3619,16 @@
       <c r="H46" s="9" t="n">
         <v>1.39583333333333</v>
       </c>
-      <c r="I46" s="18" t="n">
+      <c r="I46" s="21" t="n">
         <v>1.41666666666667</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="47">
-      <c r="A47" s="9" t="n">
-        <v>1.41666666666667</v>
-      </c>
-      <c r="B47" s="18" t="n">
-        <v>1.4375</v>
+      <c r="A47" s="18" t="n">
+        <v>41203.4166666667</v>
+      </c>
+      <c r="B47" s="19" t="n">
+        <v>41203.4375</v>
       </c>
       <c r="C47" s="11" t="s">
         <v>95</v>
@@ -3384,16 +3642,16 @@
       <c r="H47" s="9" t="n">
         <v>1.41666666666667</v>
       </c>
-      <c r="I47" s="18" t="n">
+      <c r="I47" s="21" t="n">
         <v>1.4375</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="48">
-      <c r="A48" s="9" t="n">
-        <v>1.4375</v>
-      </c>
-      <c r="B48" s="18" t="n">
-        <v>1.45833333333334</v>
+      <c r="A48" s="18" t="n">
+        <v>41203.4375</v>
+      </c>
+      <c r="B48" s="19" t="n">
+        <v>41203.4583333333</v>
       </c>
       <c r="C48" s="11" t="s">
         <v>98</v>
@@ -3413,16 +3671,16 @@
       <c r="H48" s="9" t="n">
         <v>1.4375</v>
       </c>
-      <c r="I48" s="18" t="n">
+      <c r="I48" s="21" t="n">
         <v>1.45833333333334</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="49">
-      <c r="A49" s="9" t="n">
-        <v>1.45833333333333</v>
-      </c>
-      <c r="B49" s="18" t="n">
-        <v>1.47916666666667</v>
+      <c r="A49" s="18" t="n">
+        <v>41203.4583333333</v>
+      </c>
+      <c r="B49" s="19" t="n">
+        <v>41203.4791666667</v>
       </c>
       <c r="C49" s="11" t="s">
         <v>100</v>
@@ -3436,16 +3694,16 @@
       <c r="H49" s="9" t="n">
         <v>1.45833333333333</v>
       </c>
-      <c r="I49" s="18" t="n">
+      <c r="I49" s="21" t="n">
         <v>1.47916666666667</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="50">
-      <c r="A50" s="9" t="n">
-        <v>1.47916666666667</v>
-      </c>
-      <c r="B50" s="18" t="n">
-        <v>1.5</v>
+      <c r="A50" s="18" t="n">
+        <v>41203.4791666667</v>
+      </c>
+      <c r="B50" s="19" t="n">
+        <v>41203.5</v>
       </c>
       <c r="C50" s="11" t="s">
         <v>103</v>
@@ -3465,22 +3723,22 @@
       <c r="H50" s="9" t="n">
         <v>1.47916666666667</v>
       </c>
-      <c r="I50" s="18" t="n">
+      <c r="I50" s="21" t="n">
         <v>1.5</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="51">
-      <c r="A51" s="9" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="B51" s="18" t="n">
-        <v>1.52083333333334</v>
-      </c>
-      <c r="C51" s="20" t="s">
+      <c r="A51" s="18" t="n">
+        <v>41203.5</v>
+      </c>
+      <c r="B51" s="19" t="n">
+        <v>41203.5208333333</v>
+      </c>
+      <c r="C51" s="23" t="s">
         <v>105</v>
       </c>
       <c r="D51" s="11"/>
-      <c r="E51" s="20" t="s">
+      <c r="E51" s="23" t="s">
         <v>103</v>
       </c>
       <c r="F51" s="11"/>
@@ -3488,37 +3746,45 @@
       <c r="H51" s="9" t="n">
         <v>1.5</v>
       </c>
-      <c r="I51" s="18" t="n">
+      <c r="I51" s="21" t="n">
         <v>1.52083333333334</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="52">
-      <c r="A52" s="9" t="n">
-        <v>1.52083333333333</v>
-      </c>
-      <c r="B52" s="18" t="n">
-        <v>1.54166666666667</v>
+      <c r="A52" s="18" t="n">
+        <v>41203.5208333333</v>
+      </c>
+      <c r="B52" s="19" t="n">
+        <v>41203.5416666667</v>
       </c>
       <c r="C52" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D52" s="11"/>
-      <c r="E52" s="11"/>
-      <c r="F52" s="11"/>
-      <c r="G52" s="11"/>
+      <c r="D52" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E52" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F52" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="G52" s="11" t="s">
+        <v>21</v>
+      </c>
       <c r="H52" s="9" t="n">
         <v>1.52083333333333</v>
       </c>
-      <c r="I52" s="18" t="n">
+      <c r="I52" s="21" t="n">
         <v>1.54166666666667</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="53">
-      <c r="A53" s="9" t="n">
-        <v>1.54166666666667</v>
-      </c>
-      <c r="B53" s="18" t="n">
-        <v>1.5625</v>
+      <c r="A53" s="18" t="n">
+        <v>41203.5416666667</v>
+      </c>
+      <c r="B53" s="19" t="n">
+        <v>41203.5625</v>
       </c>
       <c r="C53" s="11" t="s">
         <v>108</v>
@@ -3538,16 +3804,16 @@
       <c r="H53" s="9" t="n">
         <v>1.54166666666667</v>
       </c>
-      <c r="I53" s="18" t="n">
+      <c r="I53" s="21" t="n">
         <v>1.5625</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="54">
-      <c r="A54" s="9" t="n">
-        <v>1.5625</v>
-      </c>
-      <c r="B54" s="18" t="n">
-        <v>1.58333333333334</v>
+      <c r="A54" s="18" t="n">
+        <v>41203.5625</v>
+      </c>
+      <c r="B54" s="19" t="n">
+        <v>41203.5833333333</v>
       </c>
       <c r="C54" s="11" t="s">
         <v>109</v>
@@ -3561,16 +3827,16 @@
       <c r="H54" s="9" t="n">
         <v>1.5625</v>
       </c>
-      <c r="I54" s="18" t="n">
+      <c r="I54" s="21" t="n">
         <v>1.58333333333334</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="55">
-      <c r="A55" s="9" t="n">
-        <v>1.58333333333333</v>
-      </c>
-      <c r="B55" s="18" t="n">
-        <v>1.60416666666667</v>
+      <c r="A55" s="18" t="n">
+        <v>41203.5833333333</v>
+      </c>
+      <c r="B55" s="19" t="n">
+        <v>41203.6041666667</v>
       </c>
       <c r="C55" s="11" t="s">
         <v>112</v>
@@ -3590,16 +3856,16 @@
       <c r="H55" s="9" t="n">
         <v>1.58333333333333</v>
       </c>
-      <c r="I55" s="18" t="n">
+      <c r="I55" s="21" t="n">
         <v>1.60416666666667</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="56">
-      <c r="A56" s="9" t="n">
-        <v>1.60416666666667</v>
-      </c>
-      <c r="B56" s="18" t="n">
-        <v>0.635416666666667</v>
+      <c r="A56" s="18" t="n">
+        <v>41203.6041666667</v>
+      </c>
+      <c r="B56" s="19" t="n">
+        <v>41203.6354166667</v>
       </c>
       <c r="C56" s="11" t="s">
         <v>113</v>
@@ -3613,38 +3879,43 @@
       <c r="H56" s="9" t="n">
         <v>1.60416666666667</v>
       </c>
-      <c r="I56" s="18" t="n">
+      <c r="I56" s="21" t="n">
         <v>0.635416666666667</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="57">
-      <c r="A57" s="9" t="n">
-        <v>0.635416666666667</v>
-      </c>
-      <c r="B57" s="18" t="n">
-        <v>0.645833333333333</v>
+      <c r="A57" s="18" t="n">
+        <v>41203.6354166667</v>
+      </c>
+      <c r="B57" s="19" t="n">
+        <v>41203.6458333333</v>
       </c>
       <c r="C57" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="D57" s="7"/>
-      <c r="E57" s="7"/>
-      <c r="F57" s="7"/>
-      <c r="G57" s="7"/>
+      <c r="D57" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E57" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="F57" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="G57" s="7" t="s">
+        <v>54</v>
+      </c>
       <c r="H57" s="9" t="n">
         <v>0.635416666666667</v>
       </c>
-      <c r="I57" s="18" t="n">
+      <c r="I57" s="21" t="n">
         <v>0.645833333333333</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="46">
+  <mergeCells count="34">
     <mergeCell ref="C1:H1"/>
     <mergeCell ref="C2:H2"/>
-    <mergeCell ref="C3:H3"/>
-    <mergeCell ref="C4:H6"/>
-    <mergeCell ref="C7:H8"/>
     <mergeCell ref="E10:E11"/>
     <mergeCell ref="G10:G11"/>
     <mergeCell ref="E12:E13"/>
@@ -3653,19 +3924,12 @@
     <mergeCell ref="G14:G15"/>
     <mergeCell ref="E16:E17"/>
     <mergeCell ref="G16:G17"/>
-    <mergeCell ref="C18:H19"/>
-    <mergeCell ref="C20:H21"/>
-    <mergeCell ref="C22:H23"/>
     <mergeCell ref="D25:D26"/>
     <mergeCell ref="H25:H30"/>
     <mergeCell ref="D27:D28"/>
     <mergeCell ref="D29:D30"/>
-    <mergeCell ref="C31:H35"/>
     <mergeCell ref="C36:G36"/>
     <mergeCell ref="C37:G37"/>
-    <mergeCell ref="C38:G40"/>
-    <mergeCell ref="C41:G41"/>
-    <mergeCell ref="C42:G42"/>
     <mergeCell ref="D44:D45"/>
     <mergeCell ref="F44:F45"/>
     <mergeCell ref="G44:G45"/>
@@ -3678,14 +3942,12 @@
     <mergeCell ref="D50:D51"/>
     <mergeCell ref="F50:F51"/>
     <mergeCell ref="G50:G51"/>
-    <mergeCell ref="C52:G52"/>
     <mergeCell ref="D53:D54"/>
     <mergeCell ref="F53:F54"/>
     <mergeCell ref="G53:G54"/>
     <mergeCell ref="D55:D56"/>
     <mergeCell ref="F55:F56"/>
     <mergeCell ref="G55:G56"/>
-    <mergeCell ref="C57:G57"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>